<commit_message>
updated README to outline why XLSX files are only in use, along with updating said XLSX files on Google Sheets, and further restructuring of the info to be analysed soon.
</commit_message>
<xml_diff>
--- a/playstation/output/dates_&_finances_gifts_&_subscriptions.xlsx
+++ b/playstation/output/dates_&_finances_gifts_&_subscriptions.xlsx
@@ -3,12 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="2024-04-04" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2024-04-07" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'2024-04-04'!$A$1:$G$162</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'2024-04-07'!$A$1:$G$162</definedName>
   </definedNames>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="at949tI5QaGB5NvLE2ZBScOobRp7KvBG/9/YLXLKWSY="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -548,7 +553,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="[$€]#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -559,12 +564,6 @@
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
@@ -596,24 +595,24 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -842,7 +841,7 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="7.0"/>
     <col customWidth="1" min="2" max="2" width="57.13"/>
@@ -852,7 +851,7 @@
     <col customWidth="1" min="7" max="7" width="10.38"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>213.0</v>
       </c>
@@ -898,7 +897,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2">
         <v>171.0</v>
       </c>
@@ -921,7 +920,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2">
         <v>240.0</v>
       </c>
@@ -944,7 +943,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2">
         <v>243.0</v>
       </c>
@@ -967,7 +966,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2">
         <v>238.0</v>
       </c>
@@ -990,7 +989,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2">
         <v>239.0</v>
       </c>
@@ -1013,7 +1012,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>249.0</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>260.0</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>266.0</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2">
         <v>246.0</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2">
         <v>87.0</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>88.0</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>89.0</v>
       </c>
@@ -1174,7 +1173,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2">
         <v>90.0</v>
       </c>
@@ -1197,7 +1196,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>656.0</v>
       </c>
@@ -1220,7 +1219,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>629.0</v>
       </c>
@@ -1243,7 +1242,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>593.0</v>
       </c>
@@ -1266,7 +1265,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2">
         <v>486.0</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>79.99</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2">
         <v>754.0</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>725.0</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2">
         <v>761.0</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>770.0</v>
       </c>
@@ -1381,7 +1380,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2">
         <v>708.0</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>2.0</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2">
         <v>642.0</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>749.0</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2">
         <v>809.0</v>
       </c>
@@ -1496,7 +1495,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>427.0</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>14.49</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2">
         <v>631.0</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>595.0</v>
       </c>
@@ -1565,7 +1564,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2">
         <v>792.0</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>832.0</v>
       </c>
@@ -1611,7 +1610,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2">
         <v>502.0</v>
       </c>
@@ -1634,7 +1633,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>500.0</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>358.0</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>393.0</v>
       </c>
@@ -1703,7 +1702,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2">
         <v>410.0</v>
       </c>
@@ -1726,7 +1725,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2">
         <v>345.0</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2">
         <v>295.0</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2">
         <v>902.0</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2">
         <v>923.0</v>
       </c>
@@ -1818,7 +1817,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>928.0</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2">
         <v>607.0</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>888.0</v>
       </c>
@@ -1887,7 +1886,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="2">
         <v>690.0</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>703.0</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="2">
         <v>784.0</v>
       </c>
@@ -1956,7 +1955,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>639.0</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="2">
         <v>625.0</v>
       </c>
@@ -2002,7 +2001,7 @@
         <v>49.99</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="2">
         <v>102.0</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="2">
         <v>215.0</v>
       </c>
@@ -2048,7 +2047,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="2">
         <v>275.0</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="2">
         <v>669.0</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="2">
         <v>733.0</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>5.99</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="2">
         <v>821.0</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="2">
         <v>425.0</v>
       </c>
@@ -2163,7 +2162,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="2">
         <v>793.0</v>
       </c>
@@ -2186,7 +2185,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="2">
         <v>559.0</v>
       </c>
@@ -2209,7 +2208,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="2">
         <v>530.0</v>
       </c>
@@ -2232,7 +2231,7 @@
         <v>59.99</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="2">
         <v>840.0</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="2">
         <v>560.0</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="2">
         <v>457.0</v>
       </c>
@@ -2301,7 +2300,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="2">
         <v>853.0</v>
       </c>
@@ -2324,7 +2323,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="2">
         <v>830.0</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="2">
         <v>745.0</v>
       </c>
@@ -2370,7 +2369,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="2">
         <v>771.0</v>
       </c>
@@ -2393,7 +2392,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="2">
         <v>779.0</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="2">
         <v>835.0</v>
       </c>
@@ -2439,7 +2438,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="2">
         <v>464.0</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>59.99</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="2">
         <v>503.0</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="2">
         <v>881.0</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>79.99</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="2">
         <v>850.0</v>
       </c>
@@ -2531,7 +2530,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="2">
         <v>743.0</v>
       </c>
@@ -2554,7 +2553,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="2">
         <v>813.0</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="2">
         <v>816.0</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="2">
         <v>529.0</v>
       </c>
@@ -2623,7 +2622,7 @@
         <v>59.99</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="2">
         <v>831.0</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="2">
         <v>314.0</v>
       </c>
@@ -2669,7 +2668,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="2">
         <v>912.0</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="2">
         <v>674.0</v>
       </c>
@@ -2715,7 +2714,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="2">
         <v>657.0</v>
       </c>
@@ -2738,7 +2737,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="2">
         <v>877.0</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>44.99</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="2">
         <v>833.0</v>
       </c>
@@ -2784,7 +2783,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="2">
         <v>620.0</v>
       </c>
@@ -2807,7 +2806,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="2">
         <v>282.0</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="2">
         <v>586.0</v>
       </c>
@@ -2853,7 +2852,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="2">
         <v>335.0</v>
       </c>
@@ -2876,7 +2875,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="2">
         <v>827.0</v>
       </c>
@@ -2899,7 +2898,7 @@
         <v>79.99</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="2">
         <v>663.0</v>
       </c>
@@ -2922,7 +2921,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="2">
         <v>868.0</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>49.99</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="2">
         <v>476.0</v>
       </c>
@@ -2968,7 +2967,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="2">
         <v>505.0</v>
       </c>
@@ -2991,7 +2990,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="2">
         <v>414.0</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="2">
         <v>815.0</v>
       </c>
@@ -3037,7 +3036,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="2">
         <v>917.0</v>
       </c>
@@ -3060,7 +3059,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="2">
         <v>897.0</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>44.99</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="2">
         <v>843.0</v>
       </c>
@@ -3106,7 +3105,7 @@
         <v>49.99</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="2">
         <v>441.0</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="2">
         <v>839.0</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>20.99</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="2">
         <v>869.0</v>
       </c>
@@ -3175,7 +3174,7 @@
         <v>59.99</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="2">
         <v>823.0</v>
       </c>
@@ -3198,7 +3197,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="2">
         <v>789.0</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="2">
         <v>272.0</v>
       </c>
@@ -3244,7 +3243,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="2">
         <v>879.0</v>
       </c>
@@ -3267,7 +3266,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="2">
         <v>822.0</v>
       </c>
@@ -3290,7 +3289,7 @@
         <v>54.99</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="2">
         <v>413.0</v>
       </c>
@@ -3313,7 +3312,7 @@
         <v>16.99</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="2">
         <v>794.0</v>
       </c>
@@ -3336,7 +3335,7 @@
         <v>17.99</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="2">
         <v>814.0</v>
       </c>
@@ -3359,7 +3358,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="2">
         <v>841.0</v>
       </c>
@@ -3382,7 +3381,7 @@
         <v>84.99</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="2">
         <v>236.0</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="2">
         <v>195.0</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="2">
         <v>327.0</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="2">
         <v>497.0</v>
       </c>
@@ -3474,7 +3473,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="2">
         <v>795.0</v>
       </c>
@@ -3497,7 +3496,7 @@
         <v>79.99</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="2">
         <v>878.0</v>
       </c>
@@ -3520,7 +3519,7 @@
         <v>44.99</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="2">
         <v>863.0</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="2">
         <v>905.0</v>
       </c>
@@ -3566,7 +3565,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="2">
         <v>837.0</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="2">
         <v>354.0</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>21.99</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="2">
         <v>920.0</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="2">
         <v>919.0</v>
       </c>
@@ -3658,7 +3657,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="2">
         <v>849.0</v>
       </c>
@@ -3681,7 +3680,7 @@
         <v>59.99</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="2">
         <v>866.0</v>
       </c>
@@ -3704,7 +3703,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="2">
         <v>801.0</v>
       </c>
@@ -3727,7 +3726,7 @@
         <v>74.99</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="2">
         <v>819.0</v>
       </c>
@@ -3750,7 +3749,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="2">
         <v>787.0</v>
       </c>
@@ -3773,7 +3772,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="2">
         <v>812.0</v>
       </c>
@@ -3796,7 +3795,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="2">
         <v>893.0</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="2">
         <v>403.0</v>
       </c>
@@ -3842,7 +3841,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="2">
         <v>572.0</v>
       </c>
@@ -3865,7 +3864,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="2">
         <v>501.0</v>
       </c>
@@ -3888,7 +3887,7 @@
         <v>15.99</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="2">
         <v>630.0</v>
       </c>
@@ -3911,7 +3910,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="2">
         <v>660.0</v>
       </c>
@@ -3934,7 +3933,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="2">
         <v>865.0</v>
       </c>
@@ -3957,7 +3956,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="2">
         <v>856.0</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>59.99</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="2">
         <v>818.0</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="2">
         <v>719.0</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="2">
         <v>838.0</v>
       </c>
@@ -4049,7 +4048,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="2">
         <v>509.0</v>
       </c>
@@ -4072,7 +4071,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="2">
         <v>539.0</v>
       </c>
@@ -4095,7 +4094,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="2">
         <v>412.0</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="2">
         <v>442.0</v>
       </c>
@@ -4141,7 +4140,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="2">
         <v>925.0</v>
       </c>
@@ -4164,7 +4163,7 @@
         <v>19.99</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="2">
         <v>871.0</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="2">
         <v>508.0</v>
       </c>
@@ -4210,7 +4209,7 @@
         <v>49.99</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="2">
         <v>825.0</v>
       </c>
@@ -4233,7 +4232,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="2">
         <v>926.0</v>
       </c>
@@ -4256,7 +4255,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="2">
         <v>908.0</v>
       </c>
@@ -4279,7 +4278,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="2">
         <v>862.0</v>
       </c>
@@ -4302,7 +4301,7 @@
         <v>89.99</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="2">
         <v>788.0</v>
       </c>
@@ -4325,7 +4324,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="2">
         <v>890.0</v>
       </c>
@@ -4348,7 +4347,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="2">
         <v>880.0</v>
       </c>
@@ -4371,7 +4370,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="2">
         <v>854.0</v>
       </c>
@@ -4394,7 +4393,7 @@
         <v>69.99</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="2">
         <v>857.0</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>54.99</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="2">
         <v>929.0</v>
       </c>
@@ -4440,7 +4439,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="2">
         <v>931.0</v>
       </c>
@@ -4463,7 +4462,7 @@
         <v>29.99</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="2">
         <v>932.0</v>
       </c>
@@ -4486,7 +4485,7 @@
         <v>59.99</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="2">
         <v>935.0</v>
       </c>
@@ -4509,7 +4508,7 @@
         <v>79.99</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="2">
         <v>936.0</v>
       </c>
@@ -4532,7 +4531,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="2">
         <v>940.0</v>
       </c>
@@ -4556,7 +4555,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="2">
         <v>941.0</v>
       </c>
@@ -4580,7 +4579,8 @@
         <v>16.99</v>
       </c>
     </row>
-    <row r="164">
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1">
       <c r="E164" s="8">
         <f t="shared" ref="E164:G164" si="2">SUM(E2:E162)</f>
         <v>4940.1</v>
@@ -4602,7 +4602,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" ht="15.75" customHeight="1">
       <c r="E165" s="8">
         <f>E164/I164</f>
         <v>30.68385093</v>
@@ -4624,6 +4624,841 @@
         <v>1</v>
       </c>
     </row>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="$A$1:$G$162"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
added various charts: savings, countries, developers, etc.
</commit_message>
<xml_diff>
--- a/playstation/output/dates_&_finances_gifts_&_subscriptions.xlsx
+++ b/playstation/output/dates_&_finances_gifts_&_subscriptions.xlsx
@@ -4,14 +4,15 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="2024-09-23" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="gifts" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'2024-09-23'!$A$1:$G$178</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">gifts!$A$1:$G$178</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="TX2ZcCTkVlUHDeUm07f6j7jXImeE/xKWRx8BTnRft8k="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="bBF0SmgNh1+i7fXP9o6Z+9+wMedr5bCYFxaXNQXsRy8="/>
     </ext>
   </extLst>
 </workbook>
@@ -675,6 +676,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -873,6 +878,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>